<commit_message>
Everything appears to be working.  Yea me.  Documentation next.
</commit_message>
<xml_diff>
--- a/doc/opensdl message.xlsx
+++ b/doc/opensdl message.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\OpenSDL\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F75F9F-A798-4F52-83B8-B7D31523CB4D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3A8A30-E4C8-4380-A4F7-79D54C2497F1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="18030" windowHeight="8055" xr2:uid="{B1A19320-FFB0-485E-8AA0-1B0AC214ECB9}"/>
+    <workbookView xWindow="0" yWindow="1260" windowWidth="18030" windowHeight="8055" xr2:uid="{B1A19320-FFB0-485E-8AA0-1B0AC214ECB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="160">
   <si>
     <t>#define SDL_NORMAL</t>
   </si>
@@ -507,6 +507,9 @@
   </si>
   <si>
     <t>SDL_INVQUAL</t>
+  </si>
+  <si>
+    <t>SDL_PARSEERR</t>
   </si>
 </sst>
 </file>
@@ -873,7 +876,7 @@
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:C81"/>
+      <selection activeCell="A82" sqref="A82:C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3222,18 +3225,18 @@
         <v>124</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" ref="B66:B97" si="13">TRIM(MID(A66,8,99))</f>
+        <f t="shared" ref="B66:B69" si="13">TRIM(MID(A66,8,99))</f>
         <v>SDL_BADNODETYPE</v>
       </c>
       <c r="C66" t="s">
         <v>125</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" ref="D66:D97" si="14">TRIM(MID(C66,3,8))</f>
+        <f t="shared" ref="D66:D69" si="14">TRIM(MID(C66,3,8))</f>
         <v>00ba0200</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" ref="E66:E97" si="15">MID(D66,1,1)</f>
+        <f t="shared" ref="E66:E69" si="15">MID(D66,1,1)</f>
         <v>0</v>
       </c>
       <c r="F66">
@@ -3773,31 +3776,37 @@
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>#define SDL_PARSEERR</v>
+      </c>
+      <c r="B82" t="s">
+        <v>159</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>0x00ba027a</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>00ba027a</v>
       </c>
       <c r="E82" t="str">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="F82" t="str">
+        <v>0</v>
+      </c>
+      <c r="F82">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="G82" t="str">
+        <v>186</v>
+      </c>
+      <c r="G82">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="H82" t="str">
+        <v>79</v>
+      </c>
+      <c r="H82">
         <f t="shared" si="23"/>
-        <v/>
+        <v>2</v>
+      </c>
+      <c r="I82" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cleaned up some bugs and started working on generating a list file.
</commit_message>
<xml_diff>
--- a/doc/opensdl message.xlsx
+++ b/doc/opensdl message.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\OpenSDL\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3A8A30-E4C8-4380-A4F7-79D54C2497F1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6BA63B-943F-4FC7-BB01-E66CBBD54B03}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1260" windowWidth="18030" windowHeight="8055" xr2:uid="{B1A19320-FFB0-485E-8AA0-1B0AC214ECB9}"/>
+    <workbookView xWindow="0" yWindow="1680" windowWidth="18030" windowHeight="8055" xr2:uid="{B1A19320-FFB0-485E-8AA0-1B0AC214ECB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="163">
   <si>
     <t>#define SDL_NORMAL</t>
   </si>
@@ -510,6 +510,15 @@
   </si>
   <si>
     <t>SDL_PARSEERR</t>
+  </si>
+  <si>
+    <t>SDL_CREATED</t>
+  </si>
+  <si>
+    <t>SDL_NOTCREATED</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -876,7 +885,7 @@
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:C82"/>
+      <selection activeCell="A83" sqref="A83:C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3812,61 +3821,73 @@
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>#define SDL_CREATED</v>
+      </c>
+      <c r="B83" t="s">
+        <v>160</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>0x00ba0281</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>00ba0281</v>
       </c>
       <c r="E83" t="str">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="F83" t="str">
+        <v>0</v>
+      </c>
+      <c r="F83">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="G83" t="str">
+        <v>186</v>
+      </c>
+      <c r="G83">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="H83" t="str">
+        <v>80</v>
+      </c>
+      <c r="H83">
         <f t="shared" si="23"/>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="I83" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>#define SDL_NOTCREATED</v>
+      </c>
+      <c r="B84" t="s">
+        <v>161</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>0x00ba0289</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>00ba0289</v>
       </c>
       <c r="E84" t="str">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="F84" t="str">
+        <v>0</v>
+      </c>
+      <c r="F84">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="G84" t="str">
+        <v>186</v>
+      </c>
+      <c r="G84">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="H84" t="str">
+        <v>81</v>
+      </c>
+      <c r="H84">
         <f t="shared" si="23"/>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Continued working on generating a listing file.
</commit_message>
<xml_diff>
--- a/doc/opensdl message.xlsx
+++ b/doc/opensdl message.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\OpenSDL\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6BA63B-943F-4FC7-BB01-E66CBBD54B03}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB9D975-C386-48B1-93A2-0D5EA479F298}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1680" windowWidth="18030" windowHeight="8055" xr2:uid="{B1A19320-FFB0-485E-8AA0-1B0AC214ECB9}"/>
+    <workbookView xWindow="0" yWindow="2100" windowWidth="18030" windowHeight="8055" xr2:uid="{B1A19320-FFB0-485E-8AA0-1B0AC214ECB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="164">
   <si>
     <t>#define SDL_NORMAL</t>
   </si>
@@ -519,6 +519,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>SDL_DUPLISTQUAL</t>
   </si>
 </sst>
 </file>
@@ -885,7 +888,7 @@
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:C84"/>
+      <selection activeCell="A85" sqref="A85:C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3893,31 +3896,37 @@
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>#define SDL_DUPLISTQUAL</v>
+      </c>
+      <c r="B85" t="s">
+        <v>163</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>0x00ba0292</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>00ba0292</v>
       </c>
       <c r="E85" t="str">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="F85" t="str">
+        <v>0</v>
+      </c>
+      <c r="F85">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="G85" t="str">
+        <v>186</v>
+      </c>
+      <c r="G85">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="H85" t="str">
+        <v>82</v>
+      </c>
+      <c r="H85">
         <f t="shared" si="23"/>
-        <v/>
+        <v>2</v>
+      </c>
+      <c r="I85" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Now using argp exclusively.
</commit_message>
<xml_diff>
--- a/doc/opensdl message.xlsx
+++ b/doc/opensdl message.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\OpenSDL\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB9D975-C386-48B1-93A2-0D5EA479F298}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7985E11-B813-4AB6-AA77-8872EE326C6E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2100" windowWidth="18030" windowHeight="8055" xr2:uid="{B1A19320-FFB0-485E-8AA0-1B0AC214ECB9}"/>
+    <workbookView xWindow="5820" yWindow="2010" windowWidth="21600" windowHeight="11505" xr2:uid="{B1A19320-FFB0-485E-8AA0-1B0AC214ECB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="165">
   <si>
     <t>#define SDL_NORMAL</t>
   </si>
@@ -522,6 +523,9 @@
   </si>
   <si>
     <t>SDL_DUPLISTQUAL</t>
+  </si>
+  <si>
+    <t>SDL_CONFLDUPLQ</t>
   </si>
 </sst>
 </file>
@@ -887,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A2276F-289B-43F7-8B59-7E7E061C1DDC}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85:C85"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3932,31 +3936,37 @@
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>#define SDL_CONFLDUPLQ</v>
+      </c>
+      <c r="B86" t="s">
+        <v>164</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>0x00ba029a</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>00ba029a</v>
       </c>
       <c r="E86" t="str">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="F86" t="str">
+        <v>0</v>
+      </c>
+      <c r="F86">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="G86" t="str">
+        <v>186</v>
+      </c>
+      <c r="G86">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="H86" t="str">
+        <v>83</v>
+      </c>
+      <c r="H86">
         <f t="shared" si="23"/>
-        <v/>
+        <v>2</v>
+      </c>
+      <c r="I86" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -4380,7 +4390,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H92">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H92">
     <sortCondition ref="G2:G92"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>